<commit_message>
add returning worker / trips
</commit_message>
<xml_diff>
--- a/worker.xlsx
+++ b/worker.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsbunting/side_projects/worker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B10C16-19CD-A141-883E-E5E555FF622A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49F721B-0F67-3E48-BF7C-D6E1CFDFE343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="6420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10460" yWindow="2120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="worker-2" sheetId="1" r:id="rId1"/>
+    <sheet name="harvest worker" sheetId="1" r:id="rId1"/>
+    <sheet name="returning harvest worker" sheetId="2" r:id="rId2"/>
+    <sheet name="return trip" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="worker" localSheetId="0">'worker-2'!$A$1:$Y$2</definedName>
+    <definedName name="worker" localSheetId="0">'harvest worker'!$A$1:$Y$2</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -25,7 +27,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{0809FF3D-9525-1942-9AE9-CBC6818D45A4}" name="worker" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/larsbunting/side_projects/worker/worker.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr sourceFile="/Users/larsbunting/side_projects/worker/worker.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="25">
         <textField/>
         <textField/>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -142,9 +144,6 @@
     <t>sat Sercaita, com. Sinca,</t>
   </si>
   <si>
-    <t>muss nachgetragen werden</t>
-  </si>
-  <si>
     <t>ROU</t>
   </si>
   <si>
@@ -170,13 +169,34 @@
   </si>
   <si>
     <t>blubb</t>
+  </si>
+  <si>
+    <t>steht jetzt drin</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>airplane</t>
+  </si>
+  <si>
+    <t>return_trip_date_plane</t>
+  </si>
+  <si>
+    <t>destination_airport</t>
+  </si>
+  <si>
+    <t>SFX</t>
+  </si>
+  <si>
+    <t>birthday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +335,12 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF008000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -660,11 +686,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1027,7 +1056,7 @@
   <dimension ref="A1:Y320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1135,17 +1164,14 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>77932</v>
-      </c>
       <c r="B2">
         <v>2191</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -1154,35 +1180,35 @@
         <v>507204</v>
       </c>
       <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="K2" s="1">
         <v>36451</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
         <v>13</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P2" s="1">
         <v>43976</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R2" s="2">
         <v>0.64583333333333337</v>
@@ -1194,10 +1220,10 @@
         <v>0</v>
       </c>
       <c r="X2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" t="s">
         <v>33</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
@@ -3107,6 +3133,120 @@
       <c r="J320" s="1"/>
       <c r="L320" s="2"/>
       <c r="M320" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B899814A-E0CE-4946-B16A-97CA648C7E24}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="52" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21E80C3-E71F-6A4D-8DFF-38D394B79E8E}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="6">
+        <v>43969</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1234</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43969</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
should have been DOB
</commit_message>
<xml_diff>
--- a/worker.xlsx
+++ b/worker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsbunting/side_projects/worker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49F721B-0F67-3E48-BF7C-D6E1CFDFE343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7190C99-7C20-8544-9DD2-28F85C4415E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="2120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9360" yWindow="2120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harvest worker" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -102,9 +102,6 @@
     <t>arrival_time</t>
   </si>
   <si>
-    <t>HAM</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -141,43 +138,7 @@
     <t>updated_at</t>
   </si>
   <si>
-    <t>sat Sercaita, com. Sinca,</t>
-  </si>
-  <si>
-    <t>ROU</t>
-  </si>
-  <si>
-    <t>ZV174116</t>
-  </si>
-  <si>
-    <t>Brasov</t>
-  </si>
-  <si>
-    <t>SR8121</t>
-  </si>
-  <si>
-    <t>IAS</t>
-  </si>
-  <si>
-    <t>2020-04-27T09:35:01.000000Z</t>
-  </si>
-  <si>
-    <t>2020-04-27T16:06:22.000000Z</t>
-  </si>
-  <si>
-    <t>Richtig</t>
-  </si>
-  <si>
-    <t>blubb</t>
-  </si>
-  <si>
-    <t>steht jetzt drin</t>
-  </si>
-  <si>
     <t>type</t>
-  </si>
-  <si>
-    <t>airplane</t>
   </si>
   <si>
     <t>return_trip_date_plane</t>
@@ -186,17 +147,29 @@
     <t>destination_airport</t>
   </si>
   <si>
-    <t>SFX</t>
+    <t>return</t>
   </si>
   <si>
-    <t>birthday</t>
+    <t>me</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>please</t>
+  </si>
+  <si>
+    <t>zu hause</t>
+  </si>
+  <si>
+    <t>POL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,10 +312,16 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF2FFF12"/>
+      <name val="Source Code Pro for Powerline"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Menlo"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -686,14 +665,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1055,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y320"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1088,10 +1069,10 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1100,13 +1081,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -1124,7 +1105,7 @@
         <v>6</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N1" t="s">
         <v>7</v>
@@ -1145,86 +1126,33 @@
         <v>12</v>
       </c>
       <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B2">
-        <v>2191</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1">
-        <v>507204</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="1">
-        <v>36451</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="F2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="1">
-        <v>43976</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0.71180555555555547</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="X2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>33</v>
-      </c>
+      <c r="P2" s="1"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F3" s="1"/>
@@ -3141,10 +3069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B899814A-E0CE-4946-B16A-97CA648C7E24}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3154,40 +3082,84 @@
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>1234</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2">
+        <v>123345</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1">
+        <v>31393</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3199,54 +3171,41 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="6">
-        <v>43969</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1234</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="1">
-        <v>43969</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3254,18 +3213,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3464,6 +3423,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB5B1FF-EB44-45DD-B063-8AEC57E90A64}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B07648-4B51-490E-8E77-31E1F45FCE4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3476,14 +3443,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="e413ec1d-5181-4641-9743-a51028fe8db3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB5B1FF-EB44-45DD-B063-8AEC57E90A64}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>